<commit_message>
Added lagged dep. case.
</commit_message>
<xml_diff>
--- a/output/comp_table_voiglaender.xlsx
+++ b/output/comp_table_voiglaender.xlsx
@@ -159,26 +159,26 @@
       <c r="D2" t="n">
         <v>0.9824411762496622</v>
       </c>
-      <c r="E2" t="n">
-        <v>1.0365352918631014</v>
+      <c r="E2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="F2" t="n">
         <v>0.8829153266542367</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.9384452452482624</v>
+      <c r="G2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H2" t="n">
         <v>0.6615315399166404</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.8665485642714653</v>
+      <c r="I2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J2" t="n">
         <v>0.5392155153429105</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.7836814003184378</v>
+      <c r="K2" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3">
@@ -200,20 +200,20 @@
       <c r="F3" t="n">
         <v>-0.06598721534701023</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.12451035847817786</v>
+      <c r="G3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H3" t="n">
         <v>-0.04981209976277716</v>
       </c>
-      <c r="I3" t="n">
-        <v>-0.040346313524451276</v>
+      <c r="I3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J3" t="n">
         <v>-0.04408449644549845</v>
       </c>
-      <c r="K3" t="n">
-        <v>-0.01179472575861658</v>
+      <c r="K3" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4">
@@ -235,20 +235,20 @@
       <c r="F4" t="n">
         <v>0.27430460848134247</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.8212616196346783</v>
+      <c r="G4" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H4" t="n">
         <v>0.14506710988575133</v>
       </c>
-      <c r="I4" t="n">
-        <v>1.1355318633399643</v>
+      <c r="I4" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J4" t="n">
         <v>0.14269524144743498</v>
       </c>
-      <c r="K4" t="n">
-        <v>1.3846286694523868</v>
+      <c r="K4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5">
@@ -270,20 +270,20 @@
       <c r="F5" t="n">
         <v>0.483444034103663</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.1482443149894905</v>
+      <c r="G5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H5" t="n">
         <v>0.49653371498335847</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.33799685553075065</v>
+      <c r="I5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J5" t="n">
         <v>0.5709814638407187</v>
       </c>
-      <c r="K5" t="n">
-        <v>0.5688975090723349</v>
+      <c r="K5" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6">
@@ -311,14 +311,14 @@
       <c r="H6" t="n">
         <v>0.6497928119385233</v>
       </c>
-      <c r="I6" t="n">
-        <v>0.08000235757294226</v>
+      <c r="I6" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J6" t="n">
         <v>0.742159739648124</v>
       </c>
-      <c r="K6" t="n">
-        <v>0.09889712503586401</v>
+      <c r="K6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7">
@@ -346,14 +346,14 @@
       <c r="H7" t="n">
         <v>0.08884378445326804</v>
       </c>
-      <c r="I7" t="n">
-        <v>0.0243108318095675</v>
+      <c r="I7" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J7" t="n">
         <v>0.10728147147633658</v>
       </c>
-      <c r="K7" t="n">
-        <v>0.0060637509911775425</v>
+      <c r="K7" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8">
@@ -381,14 +381,14 @@
       <c r="H8" t="n">
         <v>0.18947037277736017</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.06996880271540154</v>
+      <c r="I8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J8" t="n">
         <v>0.20618740033182045</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.07621757720460962</v>
+      <c r="K8" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>